<commit_message>
in the middle of mangling this mutha
</commit_message>
<xml_diff>
--- a/t/data-grid-sample.xlsx
+++ b/t/data-grid-sample.xlsx
@@ -49,6 +49,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -133,7 +134,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -157,6 +158,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
+        <f aca="false">8999+1</f>
         <v>9000</v>
       </c>
       <c r="C2" s="0" t="s">

</xml_diff>

<commit_message>
good enough for me
</commit_message>
<xml_diff>
--- a/t/data-grid-sample.xlsx
+++ b/t/data-grid-sample.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="data-grid-sample" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,21 +20,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t xml:space="preserve">y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">helo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thar</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t xml:space="preserve">first</t>
+  </si>
+  <si>
+    <t xml:space="preserve">things</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phirst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"derp"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a,word</t>
   </si>
   <si>
     <t xml:space="preserve">over</t>
   </si>
   <si>
-    <t xml:space="preserve">duh</t>
+    <t xml:space="preserve">duhh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">magic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fourth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row</t>
   </si>
 </sst>
 </file>
@@ -49,7 +67,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -131,15 +148,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.8"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -157,12 +177,33 @@
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <f aca="false">8999+1</f>
+      <c r="B2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="n">
         <v>9000</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>4</v>
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>